<commit_message>
Added units to input files
Signed-off-by: Erdem Gümrükcü <erdem.guemruekcue@rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/src/tutorials/simulations/inputs/example_01.xlsx
+++ b/src/tutorials/simulations/inputs/example_01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egu\SpyderProjects\_datafev\datafev\src\tutorials\simulations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egu\SpyderProjects\_datafev\datafev\src\tutorials\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fleet" sheetId="1" r:id="rId1"/>
@@ -62,12 +62,6 @@
     <t>cu_id</t>
   </si>
   <si>
-    <t>cu_p_ch_max</t>
-  </si>
-  <si>
-    <t>cu_p_ds_max</t>
-  </si>
-  <si>
     <t>cu_eff</t>
   </si>
   <si>
@@ -83,12 +77,6 @@
     <t>CC01_04</t>
   </si>
   <si>
-    <t>LB</t>
-  </si>
-  <si>
-    <t>UB</t>
-  </si>
-  <si>
     <t>V2G Allowance (kWh)</t>
   </si>
   <si>
@@ -138,6 +126,18 @@
   </si>
   <si>
     <t>p_max_ds (kW)</t>
+  </si>
+  <si>
+    <t>cu_p_ch_max (kW)</t>
+  </si>
+  <si>
+    <t>cu_p_ds_max (kW)</t>
+  </si>
+  <si>
+    <t>LB (kW)</t>
+  </si>
+  <si>
+    <t>UB (kW)</t>
   </si>
 </sst>
 </file>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,10 +567,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -588,7 +588,7 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>8</v>
@@ -600,12 +600,12 @@
         <v>10</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5">
         <v>55</v>
@@ -636,12 +636,12 @@
         <v>44569.340277777781</v>
       </c>
       <c r="N2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B3" s="5">
         <v>55</v>
@@ -672,12 +672,12 @@
         <v>44569.319444444445</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" s="5">
         <v>55</v>
@@ -708,12 +708,12 @@
         <v>44569.336805555555</v>
       </c>
       <c r="N4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5">
         <v>55</v>
@@ -744,12 +744,12 @@
         <v>44569.357638888891</v>
       </c>
       <c r="N5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="5">
         <v>55</v>
@@ -780,12 +780,12 @@
         <v>44569.34375</v>
       </c>
       <c r="N6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5">
         <v>55</v>
@@ -816,12 +816,12 @@
         <v>44569.34375</v>
       </c>
       <c r="N7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="5">
         <v>55</v>
@@ -852,12 +852,12 @@
         <v>44569.361111111109</v>
       </c>
       <c r="N8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B9" s="5">
         <v>55</v>
@@ -888,7 +888,7 @@
         <v>44569.340277777781</v>
       </c>
       <c r="N9" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -907,7 +907,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -920,18 +920,18 @@
         <v>11</v>
       </c>
       <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>11</v>
@@ -945,7 +945,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>11</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>11</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>11</v>
@@ -987,7 +987,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -1001,7 +1001,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B7">
         <v>11</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>11</v>
@@ -1050,7 +1050,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1063,10 +1065,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>